<commit_message>
uploading new switch test doc
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/SOFTWARE/HAL_LAYER/TACTILE_SWITCH/SWITCH_TEST.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/SOFTWARE/HAL_LAYER/TACTILE_SWITCH/SWITCH_TEST.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="132" windowWidth="22980" windowHeight="9468"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="20730" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Test case ID</t>
   </si>
@@ -45,36 +45,60 @@
     <t>TC_SW_01</t>
   </si>
   <si>
-    <t xml:space="preserve">  </t>
-  </si>
-  <si>
     <t xml:space="preserve">   TACTILE_u8  GetState()                                                                   </t>
   </si>
   <si>
     <t>passed</t>
-  </si>
-  <si>
-    <t>Successful transition from relesased button state to pressed state passing through debouncing state leading to led turning on</t>
-  </si>
-  <si>
-    <t>connect microcontroler to a led and to a push button.              presss the push button leading to led turning on</t>
-  </si>
-  <si>
-    <t>leds turns on after pressing the switch and off after releasing.</t>
-  </si>
-  <si>
-    <t>the led state changes to turned on  when button is pressed and turned off when button is released.</t>
   </si>
   <si>
     <t>value returned by the API(TACTILE_u8SWITCHPRESSED 1/
 TACTILE_u8SWITCHRELEASED )</t>
+  </si>
+  <si>
+    <t>connect microcontroler to a 8 led and to 8 push buttons.              presss the push buttons leading to turning on the corresponding led.</t>
+  </si>
+  <si>
+    <t>led turns on after pressing the switch and off after releasing.</t>
+  </si>
+  <si>
+    <t>leds turns on after pressing the corresponding switch and off after releasing.</t>
+  </si>
+  <si>
+    <t>the led turn on  when button is pressed and turned off when button is released.</t>
+  </si>
+  <si>
+    <t>the led state changes to be turned on  when corresponding button is pressed and turned off when button is released again.</t>
+  </si>
+  <si>
+    <t>connect microcontroler to a 3 led (state leds)and to a push button.                                   press the push button leading to released, debouncing and pressed leds turning on succesivly.</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>when button is pressed the released led state turn on then debouncing then pressed .                                        the same happens but in inverse order when switch is released again.</t>
+  </si>
+  <si>
+    <t>state leds turn on in the correct order.</t>
+  </si>
+  <si>
+    <t>connect microcontroler to a led and to a push button.              presss the push button leading to led turning on and off when released</t>
+  </si>
+  <si>
+    <t>1)examining a Successful transition of the designed switch state machine  from relesased button state to pressed state passing through debouncing state leading to coreesponding led state turning on</t>
+  </si>
+  <si>
+    <t>2)examining the API returned value to turn on a led when a single button is pressed and turning it off if released.</t>
+  </si>
+  <si>
+    <t>3)expanding test case TC_SW_01 envolving other 8 switches and 8 leds and confirm their independence from each other and proper functionality of the driver.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +110,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,7 +142,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -154,9 +185,82 @@
       <right style="thin">
         <color theme="1" tint="0.34998626667073579"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="1" tint="0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
+        <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color theme="1" tint="0.34998626667073579"/>
       </bottom>
@@ -166,7 +270,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -187,47 +291,52 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -318,7 +427,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -353,7 +461,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -529,37 +636,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="29.5546875" customWidth="1"/>
-    <col min="6" max="7" width="45.44140625" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="7" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -578,84 +685,105 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:8" ht="120" customHeight="1">
+      <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+    </row>
+    <row r="4" spans="1:8" ht="75">
+      <c r="A4" s="21"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="90" customHeight="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="E5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="G5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A3:A5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding test resources to switch test sheet
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/SOFTWARE/HAL_LAYER/TACTILE_SWITCH/SWITCH_TEST.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/SOFTWARE/HAL_LAYER/TACTILE_SWITCH/SWITCH_TEST.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Test case ID</t>
   </si>
@@ -51,54 +51,66 @@
     <t>passed</t>
   </si>
   <si>
-    <t>value returned by the API(TACTILE_u8SWITCHPRESSED 1/
+    <t>connect microcontroler to a 8 led and to 8 push buttons.              presss the push buttons leading to turning on the corresponding led.</t>
+  </si>
+  <si>
+    <t>led turns on after pressing the switch and off after releasing.</t>
+  </si>
+  <si>
+    <t>leds turns on after pressing the corresponding switch and off after releasing.</t>
+  </si>
+  <si>
+    <t>the led turn on  when button is pressed and turned off when button is released.</t>
+  </si>
+  <si>
+    <t>the led state changes to be turned on  when corresponding button is pressed and turned off when button is released again.</t>
+  </si>
+  <si>
+    <t>connect microcontroler to a 3 led (state leds)and to a push button.                                   press the push button leading to released, debouncing and pressed leds turning on succesivly.</t>
+  </si>
+  <si>
+    <t>when button is pressed the released led state turn on then debouncing then pressed .                                        the same happens but in inverse order when switch is released again.</t>
+  </si>
+  <si>
+    <t>state leds turn on in the correct order.</t>
+  </si>
+  <si>
+    <t>connect microcontroler to a led and to a push button.              presss the push button leading to led turning on and off when released</t>
+  </si>
+  <si>
+    <t>1)examining a Successful transition of the designed switch state machine  from relesased button state to pressed state passing through debouncing state leading to coreesponding led state turning on</t>
+  </si>
+  <si>
+    <t>2)examining the API returned value to turn on a led when a single button is pressed and turning it off if released.</t>
+  </si>
+  <si>
+    <t>3)expanding test case TC_SW_01 envolving other 8 switches and 8 leds and confirm their independence from each other and proper functionality of the driver.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test resources </t>
+  </si>
+  <si>
+    <t>a test code that its main purpose is to check for the connected switch and read its value to check weather its (prseed/released)</t>
+  </si>
+  <si>
+    <t>value returned by the API(TACTILE_u8SWITCHPRESSED/
 TACTILE_u8SWITCHRELEASED )</t>
   </si>
   <si>
-    <t>connect microcontroler to a 8 led and to 8 push buttons.              presss the push buttons leading to turning on the corresponding led.</t>
-  </si>
-  <si>
-    <t>led turns on after pressing the switch and off after releasing.</t>
-  </si>
-  <si>
-    <t>leds turns on after pressing the corresponding switch and off after releasing.</t>
-  </si>
-  <si>
-    <t>the led turn on  when button is pressed and turned off when button is released.</t>
-  </si>
-  <si>
-    <t>the led state changes to be turned on  when corresponding button is pressed and turned off when button is released again.</t>
-  </si>
-  <si>
-    <t>connect microcontroler to a 3 led (state leds)and to a push button.                                   press the push button leading to released, debouncing and pressed leds turning on succesivly.</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>when button is pressed the released led state turn on then debouncing then pressed .                                        the same happens but in inverse order when switch is released again.</t>
-  </si>
-  <si>
-    <t>state leds turn on in the correct order.</t>
-  </si>
-  <si>
-    <t>connect microcontroler to a led and to a push button.              presss the push button leading to led turning on and off when released</t>
-  </si>
-  <si>
-    <t>1)examining a Successful transition of the designed switch state machine  from relesased button state to pressed state passing through debouncing state leading to coreesponding led state turning on</t>
-  </si>
-  <si>
-    <t>2)examining the API returned value to turn on a led when a single button is pressed and turning it off if released.</t>
-  </si>
-  <si>
-    <t>3)expanding test case TC_SW_01 envolving other 8 switches and 8 leds and confirm their independence from each other and proper functionality of the driver.</t>
+    <t>8 tactile switches , atmega2 micro controller, and 8 leds</t>
+  </si>
+  <si>
+    <t>tactile switch , atmega32 microcontroller, and led</t>
+  </si>
+  <si>
+    <t>tactile switch ,atmega2, and led</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +129,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -296,9 +316,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -320,6 +337,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -329,14 +355,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -648,110 +671,123 @@
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="7" width="45.42578125" customWidth="1"/>
+    <col min="4" max="5" width="32.5703125" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="7" max="8" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="D1" s="2"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1"/>
       <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="120" customHeight="1">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:9" ht="120" customHeight="1">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="60">
+      <c r="A4" s="17"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="90" customHeight="1">
+      <c r="A5" s="18"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="75">
-      <c r="A4" s="21"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="7" t="s">
+      <c r="D5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="E5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="H5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="90" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="23" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>